<commit_message>
Reporte diplomados bug 2
</commit_message>
<xml_diff>
--- a/static/documentos/CONSOLIDADO RED.xlsx
+++ b/static/documentos/CONSOLIDADO RED.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -33,9 +33,6 @@
     <t>Región</t>
   </si>
   <si>
-    <t>Departamento</t>
-  </si>
-  <si>
     <t>APELLIDOS DEL DOCENTE</t>
   </si>
   <si>
@@ -570,6 +567,9 @@
   </si>
   <si>
     <t>NIVEL 2 SESION 2</t>
+  </si>
+  <si>
+    <t>Fecha</t>
   </si>
 </sst>
 </file>
@@ -1523,107 +1523,125 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="24" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1632,43 +1650,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2110,14 +2110,15 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="56.7109375" style="30" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="31" customWidth="1"/>
-    <col min="3" max="4" width="13.5703125" style="31" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="31" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="31" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" style="31" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" style="32" hidden="1" customWidth="1"/>
@@ -2150,7 +2151,7 @@
       <c r="L1" s="35"/>
       <c r="M1" s="35"/>
       <c r="N1" s="44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O1" s="44"/>
       <c r="P1" s="3"/>
@@ -2161,32 +2162,32 @@
       <c r="U1" s="3"/>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
-      <c r="X1" s="116" t="s">
+      <c r="X1" s="128" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y1" s="124"/>
+      <c r="Z1" s="124"/>
+      <c r="AA1" s="124"/>
+      <c r="AB1" s="124"/>
+      <c r="AC1" s="124"/>
+      <c r="AD1" s="124"/>
+      <c r="AE1" s="124"/>
+      <c r="AF1" s="124"/>
+      <c r="AG1" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
-      <c r="AC1" s="111"/>
-      <c r="AD1" s="111"/>
-      <c r="AE1" s="111"/>
-      <c r="AF1" s="111"/>
-      <c r="AG1" s="110" t="s">
+      <c r="AH1" s="124"/>
+      <c r="AI1" s="124"/>
+      <c r="AJ1" s="124"/>
+      <c r="AK1" s="124"/>
+      <c r="AL1" s="124"/>
+      <c r="AM1" s="124"/>
+      <c r="AN1" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="AH1" s="111"/>
-      <c r="AI1" s="111"/>
-      <c r="AJ1" s="111"/>
-      <c r="AK1" s="111"/>
-      <c r="AL1" s="111"/>
-      <c r="AM1" s="111"/>
-      <c r="AN1" s="112" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO1" s="111"/>
-      <c r="AP1" s="111"/>
-      <c r="AQ1" s="111"/>
+      <c r="AO1" s="124"/>
+      <c r="AP1" s="124"/>
+      <c r="AQ1" s="124"/>
       <c r="AR1" s="4"/>
       <c r="AS1" s="4"/>
       <c r="AT1" s="4"/>
@@ -2206,64 +2207,64 @@
       <c r="K2" s="36"/>
       <c r="L2" s="36"/>
       <c r="M2" s="36"/>
-      <c r="N2" s="107" t="s">
+      <c r="N2" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="122"/>
+      <c r="P2" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="107"/>
-      <c r="P2" s="108" t="s">
+      <c r="Q2" s="111"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="108"/>
-      <c r="R2" s="109"/>
-      <c r="S2" s="119" t="s">
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="112"/>
+      <c r="W2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="108"/>
-      <c r="U2" s="108"/>
-      <c r="V2" s="109"/>
-      <c r="W2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="X2" s="113" t="s">
+      <c r="X2" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y2" s="108"/>
+      <c r="Z2" s="108"/>
+      <c r="AA2" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="114"/>
-      <c r="Z2" s="114"/>
-      <c r="AA2" s="113" t="s">
+      <c r="AB2" s="108"/>
+      <c r="AC2" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="114"/>
-      <c r="AC2" s="113" t="s">
+      <c r="AD2" s="108"/>
+      <c r="AE2" s="108"/>
+      <c r="AF2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AD2" s="114"/>
-      <c r="AE2" s="114"/>
-      <c r="AF2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG2" s="113" t="s">
+      <c r="AG2" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH2" s="108"/>
+      <c r="AI2" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="AH2" s="114"/>
-      <c r="AI2" s="113" t="s">
+      <c r="AJ2" s="108"/>
+      <c r="AK2" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="AJ2" s="114"/>
-      <c r="AK2" s="115" t="s">
+      <c r="AL2" s="108"/>
+      <c r="AM2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AL2" s="114"/>
-      <c r="AM2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="AN2" s="115" t="s">
+      <c r="AN2" s="127" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO2" s="108"/>
+      <c r="AP2" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="AO2" s="114"/>
-      <c r="AP2" s="115" t="s">
-        <v>14</v>
-      </c>
-      <c r="AQ2" s="114"/>
+      <c r="AQ2" s="108"/>
       <c r="AR2" s="4"/>
       <c r="AS2" s="4"/>
       <c r="AT2" s="4"/>
@@ -2298,10 +2299,10 @@
       <c r="R3" s="11">
         <v>8</v>
       </c>
-      <c r="S3" s="120">
+      <c r="S3" s="113">
         <v>9</v>
       </c>
-      <c r="T3" s="121"/>
+      <c r="T3" s="114"/>
       <c r="U3" s="11">
         <v>10</v>
       </c>
@@ -2311,10 +2312,10 @@
       <c r="W3" s="10">
         <v>13</v>
       </c>
-      <c r="X3" s="127">
+      <c r="X3" s="120">
         <v>17</v>
       </c>
-      <c r="Y3" s="114"/>
+      <c r="Y3" s="108"/>
       <c r="Z3" s="11">
         <v>20</v>
       </c>
@@ -2324,10 +2325,10 @@
       <c r="AB3" s="8">
         <v>22</v>
       </c>
-      <c r="AC3" s="128">
+      <c r="AC3" s="121">
         <v>24</v>
       </c>
-      <c r="AD3" s="114"/>
+      <c r="AD3" s="108"/>
       <c r="AE3" s="10">
         <v>25</v>
       </c>
@@ -2355,14 +2356,14 @@
       <c r="AM3" s="16">
         <v>41</v>
       </c>
-      <c r="AN3" s="124">
+      <c r="AN3" s="117">
         <v>45</v>
       </c>
-      <c r="AO3" s="114"/>
-      <c r="AP3" s="125">
+      <c r="AO3" s="108"/>
+      <c r="AP3" s="118">
         <v>49</v>
       </c>
-      <c r="AQ3" s="114"/>
+      <c r="AQ3" s="108"/>
       <c r="AR3" s="4"/>
       <c r="AS3" s="4"/>
       <c r="AT3" s="4"/>
@@ -2383,85 +2384,85 @@
       <c r="L4" s="37"/>
       <c r="M4" s="37"/>
       <c r="N4" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="48" t="s">
+      <c r="P4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="29" t="s">
+      <c r="Q4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="18" t="s">
+      <c r="R4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="S4" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="122" t="s">
+      <c r="T4" s="116"/>
+      <c r="U4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="123"/>
-      <c r="U4" s="19" t="s">
+      <c r="V4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="18" t="s">
+      <c r="W4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="W4" s="18" t="s">
+      <c r="X4" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="X4" s="117" t="s">
+      <c r="Y4" s="108"/>
+      <c r="Z4" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="Y4" s="114"/>
-      <c r="Z4" s="19" t="s">
+      <c r="AA4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="AA4" s="14" t="s">
+      <c r="AB4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AB4" s="17" t="s">
+      <c r="AC4" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="AC4" s="126" t="s">
+      <c r="AD4" s="108"/>
+      <c r="AE4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AD4" s="114"/>
-      <c r="AE4" s="18" t="s">
+      <c r="AF4" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AF4" s="20" t="s">
+      <c r="AG4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="AG4" s="19" t="s">
+      <c r="AH4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AH4" s="19" t="s">
+      <c r="AI4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AI4" s="14" t="s">
+      <c r="AJ4" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AJ4" s="14" t="s">
+      <c r="AK4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AK4" s="19" t="s">
+      <c r="AL4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AL4" s="19" t="s">
+      <c r="AM4" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AM4" s="14" t="s">
+      <c r="AN4" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="AN4" s="117" t="s">
+      <c r="AO4" s="108"/>
+      <c r="AP4" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="AO4" s="114"/>
-      <c r="AP4" s="118" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ4" s="114"/>
+      <c r="AQ4" s="108"/>
       <c r="AR4" s="4"/>
       <c r="AS4" s="4"/>
       <c r="AT4" s="4"/>
@@ -2469,163 +2470,152 @@
     </row>
     <row r="5" spans="1:48" s="1" customFormat="1" ht="63" customHeight="1">
       <c r="A5" s="49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="38" t="s">
-        <v>3</v>
+      <c r="C5" s="49" t="s">
+        <v>180</v>
       </c>
       <c r="D5" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>7</v>
-      </c>
       <c r="G5" s="39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="40" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" s="40" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M5" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="W5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="X5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y5" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z5" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA5" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB5" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC5" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD5" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE5" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF5" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG5" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH5" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI5" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ5" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK5" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL5" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM5" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN5" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO5" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP5" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ5" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT5" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="AU5" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV5" s="27" t="s">
         <v>77</v>
-      </c>
-      <c r="N5" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="P5" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q5" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="R5" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="S5" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="T5" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="U5" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="V5" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="W5" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="X5" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y5" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z5" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA5" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB5" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC5" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD5" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE5" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF5" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG5" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH5" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI5" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ5" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK5" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL5" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="AM5" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN5" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO5" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP5" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="AQ5" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR5" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="AS5" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="AT5" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="AU5" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="AV5" s="27" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="AN4:AO4"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:R2"/>
     <mergeCell ref="AG1:AM1"/>
@@ -2639,6 +2629,17 @@
     <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="AP2:AQ2"/>
     <mergeCell ref="X1:AF1"/>
+    <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="AC3:AD3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2648,15 +2649,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="10" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="10" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="14" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="15.5703125" customWidth="1"/>
@@ -2679,7 +2678,7 @@
       <c r="L1" s="50"/>
       <c r="M1" s="50"/>
       <c r="N1" s="51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O1" s="52"/>
       <c r="P1" s="52"/>
@@ -2689,7 +2688,7 @@
       <c r="T1" s="52"/>
       <c r="U1" s="52"/>
       <c r="V1" s="53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W1" s="54"/>
       <c r="X1" s="54"/>
@@ -2699,21 +2698,21 @@
       <c r="AB1" s="54"/>
       <c r="AC1" s="54"/>
       <c r="AD1" s="54"/>
-      <c r="AE1" s="135" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF1" s="136"/>
-      <c r="AG1" s="136"/>
-      <c r="AH1" s="136"/>
-      <c r="AI1" s="136"/>
-      <c r="AJ1" s="136"/>
-      <c r="AK1" s="137" t="s">
-        <v>80</v>
-      </c>
-      <c r="AL1" s="130"/>
-      <c r="AM1" s="130"/>
-      <c r="AN1" s="130"/>
-      <c r="AO1" s="130"/>
+      <c r="AE1" s="129" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF1" s="130"/>
+      <c r="AG1" s="130"/>
+      <c r="AH1" s="130"/>
+      <c r="AI1" s="130"/>
+      <c r="AJ1" s="130"/>
+      <c r="AK1" s="131" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL1" s="132"/>
+      <c r="AM1" s="132"/>
+      <c r="AN1" s="132"/>
+      <c r="AO1" s="132"/>
     </row>
     <row r="2" spans="1:46" s="4" customFormat="1" ht="12.75">
       <c r="A2" s="55"/>
@@ -2730,61 +2729,61 @@
       <c r="L2" s="55"/>
       <c r="M2" s="55"/>
       <c r="N2" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="57" t="s">
         <v>13</v>
-      </c>
-      <c r="O2" s="57" t="s">
-        <v>14</v>
       </c>
       <c r="P2" s="58"/>
       <c r="Q2" s="59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R2" s="57"/>
       <c r="S2" s="57"/>
       <c r="T2" s="58"/>
       <c r="U2" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="V2" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="V2" s="138" t="s">
+      <c r="W2" s="134"/>
+      <c r="X2" s="135"/>
+      <c r="Y2" s="136" t="s">
         <v>82</v>
       </c>
-      <c r="W2" s="139"/>
-      <c r="X2" s="140"/>
-      <c r="Y2" s="141" t="s">
+      <c r="Z2" s="132"/>
+      <c r="AA2" s="132"/>
+      <c r="AB2" s="136" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC2" s="132"/>
+      <c r="AD2" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE2" s="133" t="s">
         <v>83</v>
       </c>
-      <c r="Z2" s="130"/>
-      <c r="AA2" s="130"/>
-      <c r="AB2" s="141" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC2" s="130"/>
-      <c r="AD2" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE2" s="138" t="s">
+      <c r="AF2" s="135"/>
+      <c r="AG2" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH2" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="AF2" s="140"/>
-      <c r="AG2" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH2" s="141" t="s">
+      <c r="AI2" s="132"/>
+      <c r="AJ2" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="AI2" s="130"/>
-      <c r="AJ2" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="AK2" s="141" t="s">
-        <v>13</v>
-      </c>
-      <c r="AL2" s="130"/>
-      <c r="AM2" s="130"/>
-      <c r="AN2" s="141" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO2" s="130"/>
+      <c r="AK2" s="136" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL2" s="132"/>
+      <c r="AM2" s="132"/>
+      <c r="AN2" s="136" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO2" s="132"/>
     </row>
     <row r="3" spans="1:46" s="4" customFormat="1" ht="12.75">
       <c r="A3" s="55"/>
@@ -2803,17 +2802,17 @@
       <c r="N3" s="61">
         <v>3</v>
       </c>
-      <c r="O3" s="133">
+      <c r="O3" s="138">
         <v>6</v>
       </c>
-      <c r="P3" s="130"/>
+      <c r="P3" s="132"/>
       <c r="Q3" s="62">
         <v>9</v>
       </c>
-      <c r="R3" s="134">
+      <c r="R3" s="139">
         <v>10</v>
       </c>
-      <c r="S3" s="130"/>
+      <c r="S3" s="132"/>
       <c r="T3" s="63">
         <v>11</v>
       </c>
@@ -2829,10 +2828,10 @@
       <c r="X3" s="63">
         <v>20</v>
       </c>
-      <c r="Y3" s="134">
+      <c r="Y3" s="139">
         <v>21</v>
       </c>
-      <c r="Z3" s="130"/>
+      <c r="Z3" s="132"/>
       <c r="AA3" s="63">
         <v>22</v>
       </c>
@@ -2854,22 +2853,22 @@
       <c r="AG3" s="62">
         <v>31</v>
       </c>
-      <c r="AH3" s="134">
+      <c r="AH3" s="139">
         <v>33</v>
       </c>
-      <c r="AI3" s="130"/>
+      <c r="AI3" s="132"/>
       <c r="AJ3" s="62">
         <v>35</v>
       </c>
-      <c r="AK3" s="134">
+      <c r="AK3" s="139">
         <v>39</v>
       </c>
-      <c r="AL3" s="130"/>
-      <c r="AM3" s="130"/>
-      <c r="AN3" s="134">
+      <c r="AL3" s="132"/>
+      <c r="AM3" s="132"/>
+      <c r="AN3" s="139">
         <v>43</v>
       </c>
-      <c r="AO3" s="130"/>
+      <c r="AO3" s="132"/>
     </row>
     <row r="4" spans="1:46" s="4" customFormat="1" ht="140.25">
       <c r="A4" s="55"/>
@@ -2886,227 +2885,218 @@
       <c r="L4" s="60"/>
       <c r="M4" s="60"/>
       <c r="N4" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="140" t="s">
         <v>87</v>
       </c>
-      <c r="O4" s="129" t="s">
+      <c r="P4" s="132"/>
+      <c r="Q4" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="P4" s="130"/>
-      <c r="Q4" s="65" t="s">
+      <c r="R4" s="141" t="s">
         <v>89</v>
       </c>
-      <c r="R4" s="131" t="s">
+      <c r="S4" s="132"/>
+      <c r="T4" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="S4" s="130"/>
-      <c r="T4" s="66" t="s">
+      <c r="U4" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="U4" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="V4" s="68" t="s">
+      <c r="W4" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="W4" s="69" t="s">
+      <c r="X4" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="X4" s="70" t="s">
+      <c r="Y4" s="137" t="s">
         <v>94</v>
       </c>
-      <c r="Y4" s="132" t="s">
+      <c r="Z4" s="132"/>
+      <c r="AA4" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="Z4" s="130"/>
-      <c r="AA4" s="70" t="s">
+      <c r="AB4" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="AB4" s="66" t="s">
+      <c r="AC4" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="AC4" s="70" t="s">
+      <c r="AD4" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="AD4" s="71" t="s">
+      <c r="AE4" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="AE4" s="71" t="s">
+      <c r="AF4" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="AF4" s="68" t="s">
+      <c r="AG4" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="AG4" s="65" t="s">
+      <c r="AH4" s="137" t="s">
         <v>102</v>
       </c>
-      <c r="AH4" s="132" t="s">
+      <c r="AI4" s="132"/>
+      <c r="AJ4" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="AI4" s="130"/>
-      <c r="AJ4" s="71" t="s">
+      <c r="AK4" s="137" t="s">
         <v>104</v>
       </c>
-      <c r="AK4" s="132" t="s">
+      <c r="AL4" s="132"/>
+      <c r="AM4" s="132"/>
+      <c r="AN4" s="137" t="s">
         <v>105</v>
       </c>
-      <c r="AL4" s="130"/>
-      <c r="AM4" s="130"/>
-      <c r="AN4" s="132" t="s">
-        <v>106</v>
-      </c>
-      <c r="AO4" s="130"/>
+      <c r="AO4" s="132"/>
     </row>
     <row r="5" spans="1:46" s="4" customFormat="1" ht="102">
       <c r="A5" s="79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="72" t="s">
-        <v>3</v>
+      <c r="C5" s="79" t="s">
+        <v>180</v>
       </c>
       <c r="D5" s="72" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="73" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="73" t="s">
-        <v>7</v>
-      </c>
       <c r="G5" s="73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="74" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="74" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" s="74" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L5" s="76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M5" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="P5" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="S5" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="W5" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="X5" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y5" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z5" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA5" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB5" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC5" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD5" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG5" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="AH5" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="AI5" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="AJ5" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK5" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL5" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM5" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN5" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="AO5" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR5" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS5" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT5" s="27" t="s">
         <v>77</v>
-      </c>
-      <c r="N5" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="P5" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q5" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="R5" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="S5" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="T5" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="U5" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="V5" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="W5" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="X5" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y5" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z5" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA5" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB5" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC5" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD5" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE5" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF5" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="AG5" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH5" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="AI5" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="AJ5" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK5" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL5" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="AM5" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AN5" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="AO5" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="AP5" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ5" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="AR5" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS5" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT5" s="27" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="AE1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="AN4:AO4"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="R3:S3"/>
@@ -3119,6 +3109,15 @@
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="AH4:AI4"/>
     <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="AE1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3129,14 +3128,14 @@
   <dimension ref="A1:AX5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" hidden="1" customWidth="1"/>
@@ -3180,46 +3179,46 @@
       <c r="K1" s="80"/>
       <c r="L1" s="80"/>
       <c r="M1" s="80"/>
-      <c r="N1" s="154">
+      <c r="N1" s="144">
         <v>1</v>
       </c>
-      <c r="O1" s="146"/>
-      <c r="P1" s="146"/>
-      <c r="Q1" s="146"/>
-      <c r="R1" s="146"/>
-      <c r="S1" s="146"/>
-      <c r="T1" s="146"/>
-      <c r="U1" s="146"/>
-      <c r="V1" s="146"/>
-      <c r="W1" s="146"/>
-      <c r="X1" s="146"/>
-      <c r="Y1" s="146"/>
-      <c r="Z1" s="151">
+      <c r="O1" s="143"/>
+      <c r="P1" s="143"/>
+      <c r="Q1" s="143"/>
+      <c r="R1" s="143"/>
+      <c r="S1" s="143"/>
+      <c r="T1" s="143"/>
+      <c r="U1" s="143"/>
+      <c r="V1" s="143"/>
+      <c r="W1" s="143"/>
+      <c r="X1" s="143"/>
+      <c r="Y1" s="143"/>
+      <c r="Z1" s="142">
         <v>2</v>
       </c>
-      <c r="AA1" s="146"/>
-      <c r="AB1" s="146"/>
-      <c r="AC1" s="146"/>
-      <c r="AD1" s="146"/>
-      <c r="AE1" s="146"/>
-      <c r="AF1" s="146"/>
-      <c r="AG1" s="155">
+      <c r="AA1" s="143"/>
+      <c r="AB1" s="143"/>
+      <c r="AC1" s="143"/>
+      <c r="AD1" s="143"/>
+      <c r="AE1" s="143"/>
+      <c r="AF1" s="143"/>
+      <c r="AG1" s="145">
         <v>3</v>
       </c>
-      <c r="AH1" s="146"/>
-      <c r="AI1" s="146"/>
-      <c r="AJ1" s="146"/>
-      <c r="AK1" s="146"/>
-      <c r="AL1" s="146"/>
-      <c r="AM1" s="146"/>
-      <c r="AN1" s="146"/>
-      <c r="AO1" s="146"/>
-      <c r="AP1" s="156" t="s">
-        <v>80</v>
-      </c>
-      <c r="AQ1" s="146"/>
-      <c r="AR1" s="146"/>
-      <c r="AS1" s="146"/>
+      <c r="AH1" s="143"/>
+      <c r="AI1" s="143"/>
+      <c r="AJ1" s="143"/>
+      <c r="AK1" s="143"/>
+      <c r="AL1" s="143"/>
+      <c r="AM1" s="143"/>
+      <c r="AN1" s="143"/>
+      <c r="AO1" s="143"/>
+      <c r="AP1" s="146" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ1" s="143"/>
+      <c r="AR1" s="143"/>
+      <c r="AS1" s="143"/>
     </row>
     <row r="2" spans="1:50" s="4" customFormat="1" ht="12.75">
       <c r="A2" s="55"/>
@@ -3238,65 +3237,65 @@
       <c r="N2" s="83">
         <v>1</v>
       </c>
-      <c r="O2" s="150">
+      <c r="O2" s="147">
         <v>2</v>
       </c>
-      <c r="P2" s="146"/>
-      <c r="Q2" s="151">
+      <c r="P2" s="143"/>
+      <c r="Q2" s="142">
         <v>3</v>
       </c>
-      <c r="R2" s="146"/>
-      <c r="S2" s="146"/>
-      <c r="T2" s="150">
+      <c r="R2" s="143"/>
+      <c r="S2" s="143"/>
+      <c r="T2" s="147">
         <v>4</v>
       </c>
-      <c r="U2" s="146"/>
-      <c r="V2" s="151">
+      <c r="U2" s="143"/>
+      <c r="V2" s="142">
         <v>5</v>
       </c>
-      <c r="W2" s="146"/>
-      <c r="X2" s="150">
+      <c r="W2" s="143"/>
+      <c r="X2" s="147">
         <v>6</v>
       </c>
-      <c r="Y2" s="146"/>
-      <c r="Z2" s="151">
+      <c r="Y2" s="143"/>
+      <c r="Z2" s="142">
         <v>1</v>
       </c>
-      <c r="AA2" s="146"/>
-      <c r="AB2" s="146"/>
-      <c r="AC2" s="152">
+      <c r="AA2" s="143"/>
+      <c r="AB2" s="143"/>
+      <c r="AC2" s="154">
         <v>2</v>
       </c>
-      <c r="AD2" s="153"/>
-      <c r="AE2" s="151">
+      <c r="AD2" s="155"/>
+      <c r="AE2" s="142">
         <v>3</v>
       </c>
-      <c r="AF2" s="146"/>
-      <c r="AG2" s="150">
+      <c r="AF2" s="143"/>
+      <c r="AG2" s="147">
         <v>1</v>
       </c>
-      <c r="AH2" s="146"/>
-      <c r="AI2" s="151">
+      <c r="AH2" s="143"/>
+      <c r="AI2" s="142">
         <v>2</v>
       </c>
-      <c r="AJ2" s="146"/>
-      <c r="AK2" s="150">
+      <c r="AJ2" s="143"/>
+      <c r="AK2" s="147">
         <v>3</v>
       </c>
-      <c r="AL2" s="146"/>
-      <c r="AM2" s="151">
+      <c r="AL2" s="143"/>
+      <c r="AM2" s="142">
         <v>4</v>
       </c>
-      <c r="AN2" s="146"/>
-      <c r="AO2" s="146"/>
-      <c r="AP2" s="150">
+      <c r="AN2" s="143"/>
+      <c r="AO2" s="143"/>
+      <c r="AP2" s="147">
         <v>1</v>
       </c>
-      <c r="AQ2" s="146"/>
-      <c r="AR2" s="151">
+      <c r="AQ2" s="143"/>
+      <c r="AR2" s="142">
         <v>2</v>
       </c>
-      <c r="AS2" s="146"/>
+      <c r="AS2" s="143"/>
     </row>
     <row r="3" spans="1:50" s="4" customFormat="1" ht="12.75">
       <c r="A3" s="55"/>
@@ -3315,33 +3314,33 @@
       <c r="N3" s="86">
         <v>1</v>
       </c>
-      <c r="O3" s="147">
+      <c r="O3" s="150">
         <v>3</v>
       </c>
-      <c r="P3" s="146"/>
-      <c r="Q3" s="148">
+      <c r="P3" s="143"/>
+      <c r="Q3" s="151">
         <v>5</v>
       </c>
-      <c r="R3" s="146"/>
+      <c r="R3" s="143"/>
       <c r="S3" s="87">
         <v>6</v>
       </c>
-      <c r="T3" s="149">
+      <c r="T3" s="152">
         <v>7</v>
       </c>
-      <c r="U3" s="146"/>
-      <c r="V3" s="148">
+      <c r="U3" s="143"/>
+      <c r="V3" s="151">
         <v>9</v>
       </c>
-      <c r="W3" s="146"/>
-      <c r="X3" s="147">
+      <c r="W3" s="143"/>
+      <c r="X3" s="150">
         <v>11</v>
       </c>
-      <c r="Y3" s="146"/>
-      <c r="Z3" s="145">
+      <c r="Y3" s="143"/>
+      <c r="Z3" s="153">
         <v>13</v>
       </c>
-      <c r="AA3" s="146"/>
+      <c r="AA3" s="143"/>
       <c r="AB3" s="87">
         <v>14</v>
       </c>
@@ -3351,26 +3350,26 @@
       <c r="AD3" s="89">
         <v>16</v>
       </c>
-      <c r="AE3" s="145">
+      <c r="AE3" s="153">
         <v>17</v>
       </c>
-      <c r="AF3" s="146"/>
-      <c r="AG3" s="147">
+      <c r="AF3" s="143"/>
+      <c r="AG3" s="150">
         <v>19</v>
       </c>
-      <c r="AH3" s="146"/>
-      <c r="AI3" s="145">
+      <c r="AH3" s="143"/>
+      <c r="AI3" s="153">
         <v>21</v>
       </c>
-      <c r="AJ3" s="146"/>
-      <c r="AK3" s="147">
+      <c r="AJ3" s="143"/>
+      <c r="AK3" s="150">
         <v>23</v>
       </c>
-      <c r="AL3" s="146"/>
-      <c r="AM3" s="145">
+      <c r="AL3" s="143"/>
+      <c r="AM3" s="153">
         <v>25</v>
       </c>
-      <c r="AN3" s="146"/>
+      <c r="AN3" s="143"/>
       <c r="AO3" s="87">
         <v>26</v>
       </c>
@@ -3380,10 +3379,10 @@
       <c r="AQ3" s="89">
         <v>28</v>
       </c>
-      <c r="AR3" s="145">
+      <c r="AR3" s="153">
         <v>29</v>
       </c>
-      <c r="AS3" s="146"/>
+      <c r="AS3" s="143"/>
     </row>
     <row r="4" spans="1:50" s="4" customFormat="1" ht="89.25">
       <c r="A4" s="55"/>
@@ -3400,77 +3399,77 @@
       <c r="L4" s="85"/>
       <c r="M4" s="85"/>
       <c r="N4" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="O4" s="156" t="s">
         <v>132</v>
       </c>
-      <c r="O4" s="144" t="s">
+      <c r="P4" s="149"/>
+      <c r="Q4" s="151" t="s">
         <v>133</v>
       </c>
-      <c r="P4" s="143"/>
-      <c r="Q4" s="148" t="s">
+      <c r="R4" s="149"/>
+      <c r="S4" s="91" t="s">
         <v>134</v>
       </c>
-      <c r="R4" s="143"/>
-      <c r="S4" s="91" t="s">
+      <c r="T4" s="152" t="s">
         <v>135</v>
       </c>
-      <c r="T4" s="149" t="s">
+      <c r="U4" s="149"/>
+      <c r="V4" s="151" t="s">
         <v>136</v>
       </c>
-      <c r="U4" s="143"/>
-      <c r="V4" s="148" t="s">
+      <c r="W4" s="149"/>
+      <c r="X4" s="156" t="s">
         <v>137</v>
       </c>
-      <c r="W4" s="143"/>
-      <c r="X4" s="144" t="s">
+      <c r="Y4" s="149"/>
+      <c r="Z4" s="148" t="s">
         <v>138</v>
       </c>
-      <c r="Y4" s="143"/>
-      <c r="Z4" s="142" t="s">
+      <c r="AA4" s="149"/>
+      <c r="AB4" s="92" t="s">
         <v>139</v>
       </c>
-      <c r="AA4" s="143"/>
-      <c r="AB4" s="92" t="s">
+      <c r="AC4" s="93" t="s">
         <v>140</v>
       </c>
-      <c r="AC4" s="93" t="s">
+      <c r="AD4" s="94" t="s">
         <v>141</v>
       </c>
-      <c r="AD4" s="94" t="s">
+      <c r="AE4" s="148" t="s">
         <v>142</v>
       </c>
-      <c r="AE4" s="142" t="s">
+      <c r="AF4" s="149"/>
+      <c r="AG4" s="156" t="s">
         <v>143</v>
       </c>
-      <c r="AF4" s="143"/>
-      <c r="AG4" s="144" t="s">
+      <c r="AH4" s="149"/>
+      <c r="AI4" s="148" t="s">
         <v>144</v>
       </c>
-      <c r="AH4" s="143"/>
-      <c r="AI4" s="142" t="s">
+      <c r="AJ4" s="149"/>
+      <c r="AK4" s="156" t="s">
         <v>145</v>
       </c>
-      <c r="AJ4" s="143"/>
-      <c r="AK4" s="144" t="s">
+      <c r="AL4" s="149"/>
+      <c r="AM4" s="148" t="s">
         <v>146</v>
       </c>
-      <c r="AL4" s="143"/>
-      <c r="AM4" s="142" t="s">
+      <c r="AN4" s="149"/>
+      <c r="AO4" s="92" t="s">
         <v>147</v>
       </c>
-      <c r="AN4" s="143"/>
-      <c r="AO4" s="92" t="s">
+      <c r="AP4" s="94" t="s">
         <v>148</v>
       </c>
-      <c r="AP4" s="94" t="s">
+      <c r="AQ4" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="AQ4" s="94" t="s">
+      <c r="AR4" s="148" t="s">
         <v>150</v>
       </c>
-      <c r="AR4" s="142" t="s">
-        <v>151</v>
-      </c>
-      <c r="AS4" s="143"/>
+      <c r="AS4" s="149"/>
       <c r="AT4" s="95"/>
       <c r="AU4" s="95"/>
       <c r="AV4" s="95"/>
@@ -3478,169 +3477,173 @@
     </row>
     <row r="5" spans="1:50" s="4" customFormat="1" ht="153">
       <c r="A5" s="79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="72" t="s">
-        <v>3</v>
+      <c r="C5" s="79" t="s">
+        <v>180</v>
       </c>
       <c r="D5" s="72" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="73" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="73" t="s">
-        <v>7</v>
-      </c>
       <c r="G5" s="73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="96" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="96" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" s="96" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="97" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L5" s="98" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M5" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="P5" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="W5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="X5" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y5" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z5" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA5" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB5" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC5" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE5" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF5" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG5" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AH5" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI5" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ5" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="AK5" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL5" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM5" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="AN5" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO5" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="AP5" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ5" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="AR5" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="AS5" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="AT5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="AU5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV5" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW5" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX5" s="27" t="s">
         <v>77</v>
-      </c>
-      <c r="N5" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="P5" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q5" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="R5" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="S5" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="T5" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="U5" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="V5" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="W5" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="X5" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="Y5" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z5" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="AA5" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB5" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="AC5" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD5" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="AE5" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="AF5" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG5" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="AH5" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI5" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ5" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="AK5" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="AL5" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM5" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="AN5" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO5" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP5" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="AQ5" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="AR5" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="AS5" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="AT5" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="AU5" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV5" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="AW5" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="AX5" s="27" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="AM2:AO2"/>
-    <mergeCell ref="N1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="AR3:AS3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:Y4"/>
     <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="AP2:AQ2"/>
     <mergeCell ref="AR2:AS2"/>
@@ -3657,21 +3660,17 @@
     <mergeCell ref="AG2:AH2"/>
     <mergeCell ref="AI2:AJ2"/>
     <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AM3:AN3"/>
-    <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AM2:AO2"/>
+    <mergeCell ref="N1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3689,7 +3688,7 @@
   <cols>
     <col min="1" max="1" width="42.7109375" style="104" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="105" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="106" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="106" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="106" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="106" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="106" hidden="1" customWidth="1"/>
@@ -3710,33 +3709,37 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1">
       <c r="A1" s="159" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="163" t="s">
         <v>2</v>
       </c>
+      <c r="C1" s="163" t="s">
+        <v>180</v>
+      </c>
       <c r="M1" s="160" t="s">
+        <v>175</v>
+      </c>
+      <c r="N1" s="161" t="s">
         <v>176</v>
       </c>
-      <c r="N1" s="161" t="s">
+      <c r="O1" s="161" t="s">
         <v>177</v>
       </c>
-      <c r="O1" s="161" t="s">
+      <c r="P1" s="162" t="s">
         <v>178</v>
       </c>
-      <c r="P1" s="162" t="s">
+      <c r="Q1" s="162" t="s">
         <v>179</v>
       </c>
-      <c r="Q1" s="162" t="s">
-        <v>180</v>
-      </c>
       <c r="R1" s="157" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="159"/>
       <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
       <c r="M2" s="160"/>
       <c r="N2" s="161"/>
       <c r="O2" s="161"/>
@@ -3747,6 +3750,7 @@
     <row r="3" spans="1:18">
       <c r="A3" s="159"/>
       <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
       <c r="M3" s="160"/>
       <c r="N3" s="161"/>
       <c r="O3" s="161"/>
@@ -3757,6 +3761,7 @@
     <row r="4" spans="1:18">
       <c r="A4" s="159"/>
       <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
       <c r="M4" s="160"/>
       <c r="N4" s="161"/>
       <c r="O4" s="161"/>
@@ -3767,35 +3772,33 @@
     <row r="5" spans="1:18" ht="38.25">
       <c r="A5" s="159"/>
       <c r="B5" s="163"/>
-      <c r="C5" s="99" t="s">
-        <v>3</v>
-      </c>
+      <c r="C5" s="163"/>
       <c r="D5" s="99" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="99" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" s="99" t="s">
         <v>170</v>
       </c>
-      <c r="F5" s="99" t="s">
+      <c r="G5" s="100" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="101" t="s">
         <v>171</v>
       </c>
-      <c r="G5" s="100" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="101" t="s">
+      <c r="I5" s="101" t="s">
         <v>172</v>
       </c>
-      <c r="I5" s="101" t="s">
+      <c r="J5" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="J5" s="102" t="s">
+      <c r="K5" s="97" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="103" t="s">
         <v>174</v>
-      </c>
-      <c r="K5" s="97" t="s">
-        <v>75</v>
-      </c>
-      <c r="L5" s="103" t="s">
-        <v>175</v>
       </c>
       <c r="M5" s="160"/>
       <c r="N5" s="161"/>
@@ -3805,7 +3808,7 @@
       <c r="R5" s="158"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="R1:R5"/>
     <mergeCell ref="A1:A5"/>
     <mergeCell ref="M1:M5"/>
@@ -3814,6 +3817,7 @@
     <mergeCell ref="P1:P5"/>
     <mergeCell ref="Q1:Q5"/>
     <mergeCell ref="B1:B5"/>
+    <mergeCell ref="C1:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="J5:K5 J6:J1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>